<commit_message>
Breaking down the alternates
</commit_message>
<xml_diff>
--- a/PQ_Challenge_202.xlsx
+++ b/PQ_Challenge_202.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9D3D41-9DDD-434A-97FA-8B860A9F28C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11155320-6B90-44E3-84C2-8155D7EE1CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29920" yWindow="1270" windowWidth="28800" windowHeight="15410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="40">
   <si>
     <t>Name1</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Bo Solution</t>
+  </si>
+  <si>
+    <t>=IFS(logical_test,value_if_true,...)</t>
   </si>
 </sst>
 </file>
@@ -330,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -344,6 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,7 +1209,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="863" row="9">
+  <wetp:taskpane dockstate="right" visibility="0" width="1410" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1217,10 +1221,15 @@
   <we:alternateReferences>
     <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
   </we:alternateReferences>
-  <we:properties/>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{2F8D9394-3AED-4A13-9F82-F94C30957947}&quot;}"/>
+  </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1495,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D94284C-519C-4B43-8C27-EA153D1DC854}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1723,7 +1732,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
@@ -1736,7 +1745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>36</v>
@@ -1749,7 +1758,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22:E39" ca="1">_xlfn.LET(
 _xlpm.lvl1_,_xlfn.SCAN(0,A2:A18,_xlfn.LAMBDA(_xlpm.ini,_xlpm.ro,_xlpm.ini+COUNTA(_xlpm.ro))),
@@ -1767,7 +1776,7 @@
         <v>Names</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D23" t="str">
         <f ca="1"/>
         <v>1</v>
@@ -1776,8 +1785,92 @@
         <f ca="1"/>
         <v>Thomas</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" cm="1">
+        <f t="array" aca="1" ref="G23:G39" ca="1">_xlfn.LET(
+    _xlpm.lvl1_, _xlfn.SCAN(0, A2:A18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlpm.ini + COUNTA(_xlpm.ro))),
+    _xlpm.lvl2_, _xlfn.SCAN(
+        0,
+        B2:B18,
+        _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlfn.IFS(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), COUNTA(OFFSET(_xlpm.ro, 0, 1)) &gt; 0, _xlpm.ini, TRUE, 0))
+    ),
+    _xlpm.lvl3_, _xlfn.SCAN(0, C2:C18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, IF(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), 0))),
+    _xlpm.arr_, _xlfn.HSTACK(_xlpm.lvl1_, _xlpm.lvl2_, _xlpm.lvl3_),
+    _xlpm.lvls_, _xlfn.BYROW(SUBSTITUTE(_xlpm.arr_, 0, ""), _xlfn.LAMBDA(_xlpm.ro, _xlfn.TEXTJOIN(".", , _xlpm.ro))),
+    _xlpm.names_, _xlfn.BYROW(A2:C18, _xlfn.LAMBDA(_xlpm.ro, _xlfn.CONCAT(_xlpm.ro))),
+    _xlpm.lvl1_
+)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" cm="1">
+        <f t="array" aca="1" ref="H23:H39" ca="1">_xlfn.LET(
+    _xlpm.lvl1_, _xlfn.SCAN(0, A2:A18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlpm.ini + COUNTA(_xlpm.ro))),
+    _xlpm.lvl2_, _xlfn.SCAN(
+        0,
+        B2:B18,
+        _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlfn.IFS(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), COUNTA(OFFSET(_xlpm.ro, 0, 1)) &gt; 0, _xlpm.ini, TRUE, 0))
+    ),
+    _xlpm.lvl3_, _xlfn.SCAN(0, C2:C18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, IF(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), 0))),
+    _xlpm.arr_, _xlfn.HSTACK(_xlpm.lvl1_, _xlpm.lvl2_, _xlpm.lvl3_),
+    _xlpm.lvls_, _xlfn.BYROW(SUBSTITUTE(_xlpm.arr_, 0, ""), _xlfn.LAMBDA(_xlpm.ro, _xlfn.TEXTJOIN(".", , _xlpm.ro))),
+    _xlpm.names_, _xlfn.BYROW(A2:C18, _xlfn.LAMBDA(_xlpm.ro, _xlfn.CONCAT(_xlpm.ro))),
+    _xlpm.lvl2_
+)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" cm="1">
+        <f t="array" aca="1" ref="I23:I39" ca="1">_xlfn.LET(
+    _xlpm.lvl1_, _xlfn.SCAN(0, A2:A18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlpm.ini + COUNTA(_xlpm.ro))),
+    _xlpm.lvl2_, _xlfn.SCAN(
+        0,
+        B2:B18,
+        _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlfn.IFS(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), COUNTA(OFFSET(_xlpm.ro, 0, 1)) &gt; 0, _xlpm.ini, TRUE, 0))
+    ),
+    _xlpm.lvl3_, _xlfn.SCAN(0, C2:C18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, IF(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), 0))),
+    _xlpm.arr_, _xlfn.HSTACK(_xlpm.lvl1_, _xlpm.lvl2_, _xlpm.lvl3_),
+    _xlpm.lvls_, _xlfn.BYROW(SUBSTITUTE(_xlpm.arr_, 0, ""), _xlfn.LAMBDA(_xlpm.ro, _xlfn.TEXTJOIN(".", , _xlpm.ro))),
+    _xlpm.names_, _xlfn.BYROW(A2:C18, _xlfn.LAMBDA(_xlpm.ro, _xlfn.CONCAT(_xlpm.ro))),
+    _xlpm.lvl3_
+)</f>
+        <v>0</v>
+      </c>
+      <c r="K23" cm="1">
+        <f t="array" aca="1" ref="K23:K39" ca="1">_xlfn.LET(_xlpm.lvl1_, _xlfn.SCAN(0, A2:A18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlpm.ini + --(LEN(_xlpm.ro) &gt; 0))), _xlpm.lvl2_, _xlfn.SCAN(0, B2:B18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlfn.IFS(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), COUNTA(OFFSET(_xlpm.ro, 0, 1)) &gt; 0, _xlpm.ini, TRUE, 0))), _xlpm.lvl3_, _xlfn.SCAN(0, C2:C18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, IF(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), 0))), _xlpm.arr_, _xlfn.HSTACK(_xlpm.lvl1_, _xlpm.lvl2_, _xlpm.lvl3_), _xlpm.lvls_, _xlfn.BYROW(SUBSTITUTE(_xlpm.arr_, 0, ""), _xlfn.LAMBDA(_xlpm.ro, _xlfn.TEXTJOIN(".", , _xlpm.ro))), _xlpm.names_, _xlfn.BYROW(A2:C18, _xlfn.LAMBDA(_xlpm.ro, _xlfn.CONCAT(_xlpm.ro))), _xlpm.lvl1_)</f>
+        <v>1</v>
+      </c>
+      <c r="L23" cm="1">
+        <f t="array" aca="1" ref="L23:L39" ca="1">_xlfn.LET(
+    _xlpm.lvl1_, _xlfn.SCAN(0, A2:A18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlpm.ini + COUNTA(_xlpm.ro))),
+    _xlpm.lvl2_, _xlfn.SCAN(
+        0,
+        B2:B18,
+        _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlfn.IFS(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), COUNTA(OFFSET(_xlpm.ro, 0, 1)) &gt; 0, _xlpm.ini, TRUE, 0))
+    ),
+    _xlpm.lvl3_, _xlfn.SCAN(0, C2:C18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, IF(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), 0))),
+    _xlpm.arr_, _xlfn.HSTACK(_xlpm.lvl1_, _xlpm.lvl2_, _xlpm.lvl3_),
+    _xlpm.lvls_, _xlfn.BYROW(SUBSTITUTE(_xlpm.arr_, 0, ""), _xlfn.LAMBDA(_xlpm.ro, _xlfn.TEXTJOIN(".", , _xlpm.ro))),
+    _xlpm.names_, _xlfn.BYROW(A2:C18, _xlfn.LAMBDA(_xlpm.ro, _xlfn.CONCAT(_xlpm.ro))),
+    _xlpm.lvl2_
+)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" cm="1">
+        <f t="array" aca="1" ref="M23:M39" ca="1">_xlfn.LET(
+    _xlpm.lvl1_, _xlfn.SCAN(0, A2:A18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlpm.ini + COUNTA(_xlpm.ro))),
+    _xlpm.lvl2_, _xlfn.SCAN(
+        0,
+        B2:B18,
+        _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, _xlfn.IFS(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), COUNTA(OFFSET(_xlpm.ro, 0, 1)) &gt; 0, _xlpm.ini, TRUE, 0))
+    ),
+    _xlpm.lvl3_, _xlfn.SCAN(0, C2:C18, _xlfn.LAMBDA(_xlpm.ini,_xlpm.ro, IF(COUNTA(_xlpm.ro) &gt; 0, _xlpm.ini + COUNTA(_xlpm.ro), 0))),
+    _xlpm.arr_, _xlfn.HSTACK(_xlpm.lvl1_, _xlpm.lvl2_, _xlpm.lvl3_),
+    _xlpm.lvls_, _xlfn.BYROW(SUBSTITUTE(_xlpm.arr_, 0, ""), _xlfn.LAMBDA(_xlpm.ro, _xlfn.TEXTJOIN(".", , _xlpm.ro))),
+    _xlpm.names_, _xlfn.BYROW(A2:C18, _xlfn.LAMBDA(_xlpm.ro, _xlfn.CONCAT(_xlpm.ro))),
+    _xlpm.lvl3_
+)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D24" t="str">
         <f ca="1"/>
         <v>1.1</v>
@@ -1786,8 +1879,32 @@
         <f ca="1"/>
         <v>Russell</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D25" t="str">
         <f ca="1"/>
         <v>2</v>
@@ -1796,8 +1913,32 @@
         <f ca="1"/>
         <v>Emily</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D26" t="str">
         <f ca="1"/>
         <v>2.1</v>
@@ -1806,8 +1947,32 @@
         <f ca="1"/>
         <v>Karen</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D27" t="str">
         <f ca="1"/>
         <v>2.2</v>
@@ -1816,8 +1981,32 @@
         <f ca="1"/>
         <v>Shirley</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D28" t="str">
         <f ca="1"/>
         <v>2.3</v>
@@ -1826,8 +2015,32 @@
         <f ca="1"/>
         <v>Lawrence</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="L28">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="M28">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D29" t="str">
         <f ca="1"/>
         <v>2.4</v>
@@ -1836,8 +2049,32 @@
         <f ca="1"/>
         <v>Christian</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="M29">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D30" t="str">
         <f ca="1"/>
         <v>3</v>
@@ -1846,8 +2083,32 @@
         <f ca="1"/>
         <v>Patricia</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D31" t="str">
         <f ca="1"/>
         <v>4</v>
@@ -1856,8 +2117,32 @@
         <f ca="1"/>
         <v>Billy</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="L31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D32" t="str">
         <f ca="1"/>
         <v>4.1</v>
@@ -1866,8 +2151,32 @@
         <f ca="1"/>
         <v>Thomas</v>
       </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D33" t="str">
         <f ca="1"/>
         <v>4.1.1</v>
@@ -1876,8 +2185,32 @@
         <f ca="1"/>
         <v>Virginia</v>
       </c>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D34" t="str">
         <f ca="1"/>
         <v>4.1.2</v>
@@ -1886,8 +2219,32 @@
         <f ca="1"/>
         <v>Nathan</v>
       </c>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="L34">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D35" t="str">
         <f ca="1"/>
         <v>4.1.3</v>
@@ -1896,8 +2253,32 @@
         <f ca="1"/>
         <v>Ethan</v>
       </c>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="K35">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D36" t="str">
         <f ca="1"/>
         <v>5</v>
@@ -1906,8 +2287,32 @@
         <f ca="1"/>
         <v>Lisa</v>
       </c>
-    </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="L36">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D37" t="str">
         <f ca="1"/>
         <v>5.1</v>
@@ -1916,8 +2321,32 @@
         <f ca="1"/>
         <v>Megan</v>
       </c>
-    </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="L37">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D38" t="str">
         <f ca="1"/>
         <v>5.1.1</v>
@@ -1926,8 +2355,32 @@
         <f ca="1"/>
         <v>Olivia</v>
       </c>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="L38">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D39" t="str">
         <f ca="1"/>
         <v>5.2</v>
@@ -1935,11 +2388,41 @@
       <c r="E39" t="str">
         <f ca="1"/>
         <v>Joe</v>
+      </c>
+      <c r="G39">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="H39">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="L39">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="E43" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1947,7 +2430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAE0DB4-CF86-4A45-93E0-BA224B72A60E}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -2361,4 +2844,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F8D9394-3AED-4A13-9F82-F94C30957947}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Bo's solution is taking more time to understand than it is worth
</commit_message>
<xml_diff>
--- a/PQ_Challenge_202.xlsx
+++ b/PQ_Challenge_202.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11155320-6B90-44E3-84C2-8155D7EE1CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98005E5-EE26-4E39-9562-1E057A40DA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29920" yWindow="1270" windowWidth="28800" windowHeight="15410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29920" yWindow="1270" windowWidth="28800" windowHeight="15410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -943,6 +943,84 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAEB37F5-50A9-9E1E-7847-9798B3B3F5F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4159250" y="2762250"/>
+          <a:ext cx="2438400" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> is interesting because it uses REGEX.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1506,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D94284C-519C-4B43-8C27-EA153D1DC854}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2430,17 +2508,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAE0DB4-CF86-4A45-93E0-BA224B72A60E}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2688,8 +2767,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D22" t="str" cm="1">
-        <f t="array" ref="D22:E38">_xlfn.HSTACK(
+      <c r="A22" t="str" cm="1">
+        <f t="array" ref="A22:B38">_xlfn.HSTACK(
     _xlfn.REGEXREPLACE(
         _xlfn.SCAN(
             0,
@@ -2708,135 +2787,135 @@
 )</f>
         <v>1</v>
       </c>
-      <c r="E22" t="str">
+      <c r="B22" t="str">
         <v>Thomas</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D23" t="str">
+      <c r="A23" t="str">
         <v>1.1</v>
       </c>
-      <c r="E23" t="str">
+      <c r="B23" t="str">
         <v>Russell</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D24" t="str">
+      <c r="A24" t="str">
         <v>2</v>
       </c>
-      <c r="E24" t="str">
+      <c r="B24" t="str">
         <v>Emily</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D25" t="str">
+      <c r="A25" t="str">
         <v>2.1</v>
       </c>
-      <c r="E25" t="str">
+      <c r="B25" t="str">
         <v>Karen</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D26" t="str">
+      <c r="A26" t="str">
         <v>2.2</v>
       </c>
-      <c r="E26" t="str">
+      <c r="B26" t="str">
         <v>Shirley</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D27" t="str">
+      <c r="A27" t="str">
         <v>2.3</v>
       </c>
-      <c r="E27" t="str">
+      <c r="B27" t="str">
         <v>Lawrence</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D28" t="str">
+      <c r="A28" t="str">
         <v>2.4</v>
       </c>
-      <c r="E28" t="str">
+      <c r="B28" t="str">
         <v>Christian</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D29" t="str">
+      <c r="A29" t="str">
         <v>3</v>
       </c>
-      <c r="E29" t="str">
+      <c r="B29" t="str">
         <v>Patricia</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D30" t="str">
+      <c r="A30" t="str">
         <v>4</v>
       </c>
-      <c r="E30" t="str">
+      <c r="B30" t="str">
         <v>Billy</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D31" t="str">
+      <c r="A31" t="str">
         <v>4.1</v>
       </c>
-      <c r="E31" t="str">
+      <c r="B31" t="str">
         <v>Thomas</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D32" t="str">
+      <c r="A32" t="str">
         <v>4.1.1</v>
       </c>
-      <c r="E32" t="str">
+      <c r="B32" t="str">
         <v>Virginia</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D33" t="str">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
         <v>4.1.2</v>
       </c>
-      <c r="E33" t="str">
+      <c r="B33" t="str">
         <v>Nathan</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D34" t="str">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
         <v>4.1.3</v>
       </c>
-      <c r="E34" t="str">
+      <c r="B34" t="str">
         <v>Ethan</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D35" t="str">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
         <v>5</v>
       </c>
-      <c r="E35" t="str">
+      <c r="B35" t="str">
         <v>Lisa</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D36" t="str">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
         <v>5.1</v>
       </c>
-      <c r="E36" t="str">
+      <c r="B36" t="str">
         <v>Megan</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D37" t="str">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
         <v>5.1.1</v>
       </c>
-      <c r="E37" t="str">
+      <c r="B37" t="str">
         <v>Olivia</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D38" t="str">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
         <v>5.2</v>
       </c>
-      <c r="E38" t="str">
+      <c r="B38" t="str">
         <v>Joe</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I now understand it all
</commit_message>
<xml_diff>
--- a/PQ_Challenge_202.xlsx
+++ b/PQ_Challenge_202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98005E5-EE26-4E39-9562-1E057A40DA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E4061A-9E07-44F9-8384-E7562BFFF907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29920" yWindow="1270" windowWidth="28800" windowHeight="15410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="41">
   <si>
     <t>Name1</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>=IFS(logical_test,value_if_true,...)</t>
+  </si>
+  <si>
+    <t>Requires only one entry per row.</t>
   </si>
 </sst>
 </file>
@@ -2506,15 +2509,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAE0DB4-CF86-4A45-93E0-BA224B72A60E}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.109375" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" customWidth="1"/>
@@ -2523,7 +2526,7 @@
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2552,8 +2555,12 @@
       <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <f>MATCH("*",A2:C2,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -2565,8 +2572,12 @@
       <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <f>MATCH("*",A3:C3,)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -2579,7 +2590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -2591,8 +2602,11 @@
       <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -2605,7 +2619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>15</v>
@@ -2617,8 +2631,12 @@
       <c r="F7" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <f>MATCH("*",A7:C7,)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>17</v>
@@ -2631,7 +2649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -2644,7 +2662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -2657,7 +2675,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>5</v>
@@ -2670,7 +2688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
@@ -2683,7 +2701,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
@@ -2696,7 +2714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
@@ -2709,7 +2727,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
@@ -2722,7 +2740,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>32</v>
@@ -2735,7 +2753,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5" t="s">
@@ -2748,7 +2766,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6" t="s">
         <v>36</v>
@@ -2761,12 +2779,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="str" cm="1">
         <f t="array" ref="A22:B38">_xlfn.HSTACK(
     _xlfn.REGEXREPLACE(
@@ -2790,133 +2808,198 @@
       <c r="B22" t="str">
         <v>Thomas</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F22" t="str" cm="1">
+        <f t="array" ref="F22:F38">_xlfn.SCAN(
+            0,
+            C2:C18,
+            _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                _xlfn.LET(
+                    _xlpm.n, MATCH("*", _xlfn.TAKE(A18:_xlpm.v, 1), ),
+                    LEFT(_xlpm.a, _xlpm.n - 1) &amp; (0 &amp; MID(_xlpm.a, _xlpm.n, 1)) + 1
+                )
+            )
+        )</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <v>1.1</v>
       </c>
       <c r="B23" t="str">
         <v>Russell</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" t="str">
+        <v>11</v>
+      </c>
+      <c r="H23">
+        <f>MATCH("T*",A2:A18,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <v>2</v>
       </c>
       <c r="B24" t="str">
         <v>Emily</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F24" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <v>2.1</v>
       </c>
       <c r="B25" t="str">
         <v>Karen</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F25" t="str">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <v>2.2</v>
       </c>
       <c r="B26" t="str">
         <v>Shirley</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F26" t="str">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <v>2.3</v>
       </c>
       <c r="B27" t="str">
         <v>Lawrence</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F27" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <v>2.4</v>
       </c>
       <c r="B28" t="str">
         <v>Christian</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F28" t="str">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <v>3</v>
       </c>
       <c r="B29" t="str">
         <v>Patricia</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F29" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <v>4</v>
       </c>
       <c r="B30" t="str">
         <v>Billy</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F30" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <v>4.1</v>
       </c>
       <c r="B31" t="str">
         <v>Thomas</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F31" t="str">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <v>4.1.1</v>
       </c>
       <c r="B32" t="str">
         <v>Virginia</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F32" t="str">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <v>4.1.2</v>
       </c>
       <c r="B33" t="str">
         <v>Nathan</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F33" t="str">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <v>4.1.3</v>
       </c>
       <c r="B34" t="str">
         <v>Ethan</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F34" t="str">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <v>5</v>
       </c>
       <c r="B35" t="str">
         <v>Lisa</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F35" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <v>5.1</v>
       </c>
       <c r="B36" t="str">
         <v>Megan</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F36" t="str">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <v>5.1.1</v>
       </c>
       <c r="B37" t="str">
         <v>Olivia</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F37" t="str">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <v>5.2</v>
       </c>
       <c r="B38" t="str">
         <v>Joe</v>
+      </c>
+      <c r="F38" t="str">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>